<commit_message>
- Inserçao da funcão de remoção de registro - Correção de falhas na coluna Data do Registro
</commit_message>
<xml_diff>
--- a/datasets/usuarios/02945327902/02945327902_dados_individuais.xlsx
+++ b/datasets/usuarios/02945327902/02945327902_dados_individuais.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,11 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -60,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +483,16 @@
           <t>Gordura Visceral</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Percentual de Gordura Corporal</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Percentual de Musculatura Corporal</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -515,6 +522,8 @@
       <c r="I2" t="n">
         <v>18</v>
       </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -544,6 +553,8 @@
       <c r="I3" t="n">
         <v>18</v>
       </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -573,6 +584,8 @@
       <c r="I4" t="n">
         <v>17</v>
       </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -602,6 +615,8 @@
       <c r="I5" t="n">
         <v>17</v>
       </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -631,6 +646,8 @@
       <c r="I6" t="n">
         <v>17</v>
       </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -660,6 +677,8 @@
       <c r="I7" t="n">
         <v>16</v>
       </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -689,6 +708,8 @@
       <c r="I8" t="n">
         <v>16</v>
       </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -718,6 +739,8 @@
       <c r="I9" t="n">
         <v>16</v>
       </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -747,6 +770,8 @@
       <c r="I10" t="n">
         <v>16</v>
       </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -776,6 +801,8 @@
       <c r="I11" t="n">
         <v>15</v>
       </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -805,6 +832,8 @@
       <c r="I12" t="n">
         <v>15</v>
       </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -834,6 +863,8 @@
       <c r="I13" t="n">
         <v>14</v>
       </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -863,12 +894,14 @@
       <c r="I14" t="n">
         <v>14</v>
       </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45770.47045805353</v>
-      </c>
-      <c r="B15" s="3" t="n">
+        <v>45770.47045805556</v>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>45770</v>
       </c>
       <c r="C15" t="n">
@@ -892,6 +925,8 @@
       <c r="I15" t="n">
         <v>14</v>
       </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>